<commit_message>
Created System1_Extract_ClientInformation and System1_Update_WorkItem workflows for client data extraction and work item updates
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\REF_CSH_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A576B3E3-9FC7-48D4-8261-57DB69D18BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8059288F-80C4-4E36-B303-8DB15949B059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>Work Item url for ACME Details URL for ACME Sytem</t>
+  </si>
+  <si>
+    <t>HashURL</t>
+  </si>
+  <si>
+    <t>ACME_WorkItemsUpdateURL</t>
   </si>
 </sst>
 </file>
@@ -2830,8 +2836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2934,8 +2940,34 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updated the code to click for update Details
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\REF_CSH_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8059288F-80C4-4E36-B303-8DB15949B059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601F06EB-22DC-4A5E-8361-F1C13CB962E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2837,7 +2837,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>